<commit_message>
aggiunta percorso di salvataggio per il file excel
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -9,12 +9,13 @@
     <sheet name="query1" r:id="rId3" sheetId="1"/>
     <sheet name="query2" r:id="rId4" sheetId="2"/>
     <sheet name="query6" r:id="rId5" sheetId="3"/>
+    <sheet name="query7" r:id="rId6" sheetId="4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="85">
   <si>
     <t>nome</t>
   </si>
@@ -266,6 +267,9 @@
   </si>
   <si>
     <t>Verdi</t>
+  </si>
+  <si>
+    <t>Vasco</t>
   </si>
 </sst>
 </file>
@@ -981,4 +985,33 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>